<commit_message>
Improve system to prevent duplicate passenger report generation
Refactor `processConsolidatedPax` to `processConsolidatedPaxForSingleShip` in `server/routes.ts` to prevent race conditions and duplicate PAX report entries.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a3af5c32-fe94-463b-bafd-8d7cf4140d74
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d67b414c-7ba7-46ed-90da-331e0aa9efb6/a3af5c32-fe94-463b-bafd-8d7cf4140d74/ISXweQc
</commit_message>
<xml_diff>
--- a/output/ship-b/eod_1757671798062.xlsx
+++ b/output/ship-b/eod_1757671798062.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
   <si>
     <t>TOUR OPERATOR REPORT</t>
   </si>
@@ -1584,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q248"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C7" sqref="C7"/>
@@ -1887,7 +1887,7 @@
       <c r="H21" s="56"/>
     </row>
     <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" ht="36" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
         <v>31</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="G23" s="58"/>
       <c r="H23" s="59"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>33</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="62"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="60"/>
       <c r="B25" s="8"/>
       <c r="C25" s="63">
@@ -1935,7 +1935,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="62"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="60"/>
       <c r="B26" s="8"/>
       <c r="C26" s="63"/>
@@ -1945,7 +1945,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="62"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="64" t="s">
         <v>37</v>
       </c>
@@ -1957,7 +1957,7 @@
       <c r="G27" s="65"/>
       <c r="H27" s="66"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="67" t="s">
         <v>38</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="G28" s="68"/>
       <c r="H28" s="69"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="70"/>
       <c r="B29" s="71"/>
       <c r="C29" s="71"/>
@@ -1979,7 +1979,7 @@
       <c r="G29" s="71"/>
       <c r="H29" s="72"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="70"/>
       <c r="B30" s="71"/>
       <c r="C30" s="71"/>
@@ -1989,7 +1989,7 @@
       <c r="G30" s="71"/>
       <c r="H30" s="72"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="70"/>
       <c r="B31" s="71"/>
       <c r="C31" s="71"/>
@@ -1999,7 +1999,7 @@
       <c r="G31" s="71"/>
       <c r="H31" s="72"/>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="70"/>
       <c r="B32" s="71"/>
       <c r="C32" s="71"/>
@@ -2009,7 +2009,7 @@
       <c r="G32" s="71"/>
       <c r="H32" s="72"/>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="60"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2023,7 +2023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
         <v>41</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="B35" s="8"/>
       <c r="C35" s="61"/>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="H35" s="77"/>
     </row>
-    <row r="36" ht="15.6" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" ht="15.6" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="B36" s="8"/>
       <c r="C36" s="61"/>
@@ -2061,7 +2061,7 @@
       <c r="G36" s="76"/>
       <c r="H36" s="78"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>33</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="G37" s="76"/>
       <c r="H37" s="79"/>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="80"/>
       <c r="B38" s="81"/>
       <c r="C38" s="82" t="s">
@@ -2099,6 +2099,7 @@
         <v>49</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="57" t="s">
         <v>31</v>
@@ -2140,7 +2141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
         <v>33</v>
       </c>
@@ -2158,7 +2159,7 @@
       <c r="G41" s="8"/>
       <c r="H41" s="62"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="B42" s="8"/>
       <c r="C42" s="63">
@@ -2174,7 +2175,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="62"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="B43" s="8"/>
       <c r="C43" s="63"/>
@@ -2184,7 +2185,7 @@
       <c r="G43" s="8"/>
       <c r="H43" s="62"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="86" t="s">
         <v>37</v>
       </c>
@@ -2196,7 +2197,7 @@
       <c r="G44" s="86"/>
       <c r="H44" s="86"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="87" t="s">
         <v>52</v>
       </c>
@@ -2208,7 +2209,7 @@
       <c r="G45" s="87"/>
       <c r="H45" s="87"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="87"/>
       <c r="B46" s="87"/>
       <c r="C46" s="87"/>
@@ -2218,7 +2219,7 @@
       <c r="G46" s="87"/>
       <c r="H46" s="87"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="87"/>
       <c r="B47" s="87"/>
       <c r="C47" s="87"/>
@@ -2228,7 +2229,7 @@
       <c r="G47" s="87"/>
       <c r="H47" s="87"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="87"/>
       <c r="B48" s="87"/>
       <c r="C48" s="87"/>
@@ -2238,7 +2239,7 @@
       <c r="G48" s="87"/>
       <c r="H48" s="87"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="87"/>
       <c r="B49" s="87"/>
       <c r="C49" s="87"/>
@@ -2248,7 +2249,7 @@
       <c r="G49" s="87"/>
       <c r="H49" s="87"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="60"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -2262,7 +2263,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="60" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="60"/>
       <c r="B52" s="8"/>
       <c r="C52" s="61"/>
@@ -2290,7 +2291,7 @@
       </c>
       <c r="H52" s="77"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="60"/>
       <c r="B53" s="8"/>
       <c r="C53" s="61"/>
@@ -2300,7 +2301,7 @@
       <c r="G53" s="76"/>
       <c r="H53" s="78"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="60" t="s">
         <v>33</v>
       </c>
@@ -2318,7 +2319,7 @@
       <c r="G54" s="76"/>
       <c r="H54" s="79"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="80"/>
       <c r="B55" s="81"/>
       <c r="C55" s="82" t="s">
@@ -2338,7 +2339,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="57" t="s">
         <v>31</v>
@@ -2380,7 +2381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="60" t="s">
         <v>33</v>
       </c>
@@ -2398,7 +2399,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="62"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
       <c r="B59" s="8"/>
       <c r="C59" s="63">
@@ -2414,7 +2415,7 @@
       <c r="G59" s="8"/>
       <c r="H59" s="62"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="60"/>
       <c r="B60" s="8"/>
       <c r="C60" s="63"/>
@@ -2424,7 +2425,7 @@
       <c r="G60" s="8"/>
       <c r="H60" s="62"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="86" t="s">
         <v>37</v>
       </c>
@@ -2436,7 +2437,7 @@
       <c r="G61" s="86"/>
       <c r="H61" s="86"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="87" t="s">
         <v>38</v>
       </c>
@@ -2448,7 +2449,7 @@
       <c r="G62" s="87"/>
       <c r="H62" s="87"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="87"/>
       <c r="B63" s="87"/>
       <c r="C63" s="87"/>
@@ -2458,7 +2459,7 @@
       <c r="G63" s="87"/>
       <c r="H63" s="87"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="87"/>
       <c r="B64" s="87"/>
       <c r="C64" s="87"/>
@@ -2468,7 +2469,7 @@
       <c r="G64" s="87"/>
       <c r="H64" s="87"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="87"/>
       <c r="B65" s="87"/>
       <c r="C65" s="87"/>
@@ -2478,7 +2479,7 @@
       <c r="G65" s="87"/>
       <c r="H65" s="87"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="87"/>
       <c r="B66" s="87"/>
       <c r="C66" s="87"/>
@@ -2488,7 +2489,7 @@
       <c r="G66" s="87"/>
       <c r="H66" s="87"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="60"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -2502,7 +2503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="60" t="s">
         <v>41</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="60"/>
       <c r="B69" s="8"/>
       <c r="C69" s="61"/>
@@ -2530,7 +2531,7 @@
       </c>
       <c r="H69" s="77"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="60"/>
       <c r="B70" s="8"/>
       <c r="C70" s="61"/>
@@ -2540,7 +2541,7 @@
       <c r="G70" s="76"/>
       <c r="H70" s="78"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="60" t="s">
         <v>33</v>
       </c>
@@ -2558,7 +2559,7 @@
       <c r="G71" s="76"/>
       <c r="H71" s="79"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="80"/>
       <c r="B72" s="81"/>
       <c r="C72" s="82" t="s">
@@ -2578,8 +2579,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="88" t="s">
         <v>54</v>
       </c>
@@ -2591,7 +2592,7 @@
       <c r="G74" s="89"/>
       <c r="H74" s="89"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="92"/>
       <c r="B75" s="92"/>
       <c r="C75" s="92"/>
@@ -2601,7 +2602,7 @@
       <c r="G75" s="92"/>
       <c r="H75" s="92"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="93"/>
       <c r="B76" s="89"/>
       <c r="C76" s="61" t="s">
@@ -2617,7 +2618,7 @@
       <c r="G76" s="89"/>
       <c r="H76" s="89"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="94" t="s">
         <v>55</v>
       </c>
@@ -2637,10 +2638,767 @@
       <c r="G77" s="95"/>
       <c r="H77" s="95"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="85"/>
+      <c r="D83" s="85"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="85"/>
+      <c r="H83" s="85"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="62"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="60"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="63">
+        <v>66</v>
+      </c>
+      <c r="D85" s="63">
+        <v>5</v>
+      </c>
+      <c r="E85" s="63">
+        <v>1</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="62"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="60"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="63"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="62"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" s="86"/>
+      <c r="C87" s="86"/>
+      <c r="D87" s="86"/>
+      <c r="E87" s="86"/>
+      <c r="F87" s="86"/>
+      <c r="G87" s="86"/>
+      <c r="H87" s="86"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="87"/>
+      <c r="C88" s="87"/>
+      <c r="D88" s="87"/>
+      <c r="E88" s="87"/>
+      <c r="F88" s="87"/>
+      <c r="G88" s="87"/>
+      <c r="H88" s="87"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="87"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="87"/>
+      <c r="D89" s="87"/>
+      <c r="E89" s="87"/>
+      <c r="F89" s="87"/>
+      <c r="G89" s="87"/>
+      <c r="H89" s="87"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="87"/>
+      <c r="B90" s="87"/>
+      <c r="C90" s="87"/>
+      <c r="D90" s="87"/>
+      <c r="E90" s="87"/>
+      <c r="F90" s="87"/>
+      <c r="G90" s="87"/>
+      <c r="H90" s="87"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="87"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="87"/>
+      <c r="D91" s="87"/>
+      <c r="E91" s="87"/>
+      <c r="F91" s="87"/>
+      <c r="G91" s="87"/>
+      <c r="H91" s="87"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="87"/>
+      <c r="B92" s="87"/>
+      <c r="C92" s="87"/>
+      <c r="D92" s="87"/>
+      <c r="E92" s="87"/>
+      <c r="F92" s="87"/>
+      <c r="G92" s="87"/>
+      <c r="H92" s="87"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="60"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H93" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="75"/>
+      <c r="G94" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H94" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="60"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="61"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="61"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H95" s="77"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="60"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="61"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="61"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="78"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E97" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="G97" s="76"/>
+      <c r="H97" s="79"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="80"/>
+      <c r="B98" s="81"/>
+      <c r="C98" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D98" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E98" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F98" s="81"/>
+      <c r="G98" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H98" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B99" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" s="85"/>
+      <c r="D99" s="85"/>
+      <c r="E99" s="85"/>
+      <c r="F99" s="85"/>
+      <c r="G99" s="85"/>
+      <c r="H99" s="85"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D100" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E100" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="62"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="60"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="63">
+        <v>72</v>
+      </c>
+      <c r="D101" s="63">
+        <v>2</v>
+      </c>
+      <c r="E101" s="63">
+        <v>1</v>
+      </c>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="62"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="60"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="62"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B103" s="86"/>
+      <c r="C103" s="86"/>
+      <c r="D103" s="86"/>
+      <c r="E103" s="86"/>
+      <c r="F103" s="86"/>
+      <c r="G103" s="86"/>
+      <c r="H103" s="86"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B104" s="87"/>
+      <c r="C104" s="87"/>
+      <c r="D104" s="87"/>
+      <c r="E104" s="87"/>
+      <c r="F104" s="87"/>
+      <c r="G104" s="87"/>
+      <c r="H104" s="87"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="87"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="87"/>
+      <c r="D105" s="87"/>
+      <c r="E105" s="87"/>
+      <c r="F105" s="87"/>
+      <c r="G105" s="87"/>
+      <c r="H105" s="87"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="87"/>
+      <c r="B106" s="87"/>
+      <c r="C106" s="87"/>
+      <c r="D106" s="87"/>
+      <c r="E106" s="87"/>
+      <c r="F106" s="87"/>
+      <c r="G106" s="87"/>
+      <c r="H106" s="87"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="87"/>
+      <c r="B107" s="87"/>
+      <c r="C107" s="87"/>
+      <c r="D107" s="87"/>
+      <c r="E107" s="87"/>
+      <c r="F107" s="87"/>
+      <c r="G107" s="87"/>
+      <c r="H107" s="87"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="87"/>
+      <c r="B108" s="87"/>
+      <c r="C108" s="87"/>
+      <c r="D108" s="87"/>
+      <c r="E108" s="87"/>
+      <c r="F108" s="87"/>
+      <c r="G108" s="87"/>
+      <c r="H108" s="87"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="60"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="G109" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H109" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="75"/>
+      <c r="G110" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H110" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="60"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="61"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="61"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H111" s="77"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="60"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="61"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="61"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="76"/>
+      <c r="H112" s="78"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D113" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E113" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F113" s="8"/>
+      <c r="G113" s="76"/>
+      <c r="H113" s="79"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="80"/>
+      <c r="B114" s="81"/>
+      <c r="C114" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D114" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F114" s="81"/>
+      <c r="G114" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H114" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" s="85"/>
+      <c r="D115" s="85"/>
+      <c r="E115" s="85"/>
+      <c r="F115" s="85"/>
+      <c r="G115" s="85"/>
+      <c r="H115" s="85"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" s="8"/>
+      <c r="C116" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D116" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E116" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="62"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="60"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="63">
+        <v>74</v>
+      </c>
+      <c r="D117" s="63">
+        <v>3</v>
+      </c>
+      <c r="E117" s="63">
+        <v>0</v>
+      </c>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="62"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="60"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="63"/>
+      <c r="D118" s="63"/>
+      <c r="E118" s="63"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="62"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B119" s="86"/>
+      <c r="C119" s="86"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
+      <c r="G119" s="86"/>
+      <c r="H119" s="86"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" s="87"/>
+      <c r="C120" s="87"/>
+      <c r="D120" s="87"/>
+      <c r="E120" s="87"/>
+      <c r="F120" s="87"/>
+      <c r="G120" s="87"/>
+      <c r="H120" s="87"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="87"/>
+      <c r="B121" s="87"/>
+      <c r="C121" s="87"/>
+      <c r="D121" s="87"/>
+      <c r="E121" s="87"/>
+      <c r="F121" s="87"/>
+      <c r="G121" s="87"/>
+      <c r="H121" s="87"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="87"/>
+      <c r="B122" s="87"/>
+      <c r="C122" s="87"/>
+      <c r="D122" s="87"/>
+      <c r="E122" s="87"/>
+      <c r="F122" s="87"/>
+      <c r="G122" s="87"/>
+      <c r="H122" s="87"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="87"/>
+      <c r="B123" s="87"/>
+      <c r="C123" s="87"/>
+      <c r="D123" s="87"/>
+      <c r="E123" s="87"/>
+      <c r="F123" s="87"/>
+      <c r="G123" s="87"/>
+      <c r="H123" s="87"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="87"/>
+      <c r="B124" s="87"/>
+      <c r="C124" s="87"/>
+      <c r="D124" s="87"/>
+      <c r="E124" s="87"/>
+      <c r="F124" s="87"/>
+      <c r="G124" s="87"/>
+      <c r="H124" s="87"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="60"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="8"/>
+      <c r="G125" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H125" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B126" s="8"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="75"/>
+      <c r="G126" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H126" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="60"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H127" s="77"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="60"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+      <c r="F128" s="8"/>
+      <c r="G128" s="76"/>
+      <c r="H128" s="78"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B129" s="8"/>
+      <c r="C129" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D129" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E129" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="8"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="79"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="80"/>
+      <c r="B130" s="81"/>
+      <c r="C130" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D130" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E130" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F130" s="81"/>
+      <c r="G130" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H130" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="33">
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
@@ -2665,6 +3423,15 @@
     <mergeCell ref="A61:H61"/>
     <mergeCell ref="A62:H66"/>
     <mergeCell ref="C68:F68"/>
+    <mergeCell ref="B83:H83"/>
+    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A88:H92"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="A103:H103"/>
+    <mergeCell ref="A104:H108"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="A120:H124"/>
   </mergeCells>
   <conditionalFormatting sqref="A28">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">

</xml_diff>

<commit_message>
Improve report generation and file handling across multiple ships
Updates existing Excel reports and generates new consolidated passenger and dispatch reports for various ships, alongside edited dispatch files.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a3af5c32-fe94-463b-bafd-8d7cf4140d74
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d67b414c-7ba7-46ed-90da-331e0aa9efb6/a3af5c32-fe94-463b-bafd-8d7cf4140d74/ISXweQc
</commit_message>
<xml_diff>
--- a/output/ship-b/eod_1757671798062.xlsx
+++ b/output/ship-b/eod_1757671798062.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="56">
   <si>
     <t>TOUR OPERATOR REPORT</t>
   </si>
@@ -2643,7 +2643,7 @@
     <row r="80" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="57" t="s">
         <v>31</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="G83" s="85"/>
       <c r="H83" s="85"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="60" t="s">
         <v>33</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="G84" s="8"/>
       <c r="H84" s="62"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="60"/>
       <c r="B85" s="8"/>
       <c r="C85" s="63">
@@ -2755,7 +2755,7 @@
       <c r="G91" s="87"/>
       <c r="H91" s="87"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="87"/>
       <c r="B92" s="87"/>
       <c r="C92" s="87"/>
@@ -2765,7 +2765,7 @@
       <c r="G92" s="87"/>
       <c r="H92" s="87"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="60"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -2779,7 +2779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="60" t="s">
         <v>41</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="60"/>
       <c r="B95" s="8"/>
       <c r="C95" s="61"/>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="H95" s="77"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="60"/>
       <c r="B96" s="8"/>
       <c r="C96" s="61"/>
@@ -2817,7 +2817,7 @@
       <c r="G96" s="76"/>
       <c r="H96" s="78"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="60" t="s">
         <v>33</v>
       </c>
@@ -2835,7 +2835,7 @@
       <c r="G97" s="76"/>
       <c r="H97" s="79"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="80"/>
       <c r="B98" s="81"/>
       <c r="C98" s="82" t="s">
@@ -2855,7 +2855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="57" t="s">
         <v>31</v>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="G99" s="85"/>
       <c r="H99" s="85"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="60" t="s">
         <v>33</v>
       </c>
@@ -2887,7 +2887,7 @@
       <c r="G100" s="8"/>
       <c r="H100" s="62"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="60"/>
       <c r="B101" s="8"/>
       <c r="C101" s="63">
@@ -2903,7 +2903,7 @@
       <c r="G101" s="8"/>
       <c r="H101" s="62"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="60"/>
       <c r="B102" s="8"/>
       <c r="C102" s="63"/>
@@ -2913,7 +2913,7 @@
       <c r="G102" s="8"/>
       <c r="H102" s="62"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="86" t="s">
         <v>37</v>
       </c>
@@ -2925,7 +2925,7 @@
       <c r="G103" s="86"/>
       <c r="H103" s="86"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="87" t="s">
         <v>52</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="G104" s="87"/>
       <c r="H104" s="87"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="87"/>
       <c r="B105" s="87"/>
       <c r="C105" s="87"/>
@@ -2947,7 +2947,7 @@
       <c r="G105" s="87"/>
       <c r="H105" s="87"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="87"/>
       <c r="B106" s="87"/>
       <c r="C106" s="87"/>
@@ -2957,7 +2957,7 @@
       <c r="G106" s="87"/>
       <c r="H106" s="87"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="87"/>
       <c r="B107" s="87"/>
       <c r="C107" s="87"/>
@@ -2967,7 +2967,7 @@
       <c r="G107" s="87"/>
       <c r="H107" s="87"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="87"/>
       <c r="B108" s="87"/>
       <c r="C108" s="87"/>
@@ -2977,7 +2977,7 @@
       <c r="G108" s="87"/>
       <c r="H108" s="87"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="60"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
@@ -2991,7 +2991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="60" t="s">
         <v>41</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="60"/>
       <c r="B111" s="8"/>
       <c r="C111" s="61"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="H111" s="77"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="60"/>
       <c r="B112" s="8"/>
       <c r="C112" s="61"/>
@@ -3029,7 +3029,7 @@
       <c r="G112" s="76"/>
       <c r="H112" s="78"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="60" t="s">
         <v>33</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="G113" s="76"/>
       <c r="H113" s="79"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="80"/>
       <c r="B114" s="81"/>
       <c r="C114" s="82" t="s">
@@ -3067,7 +3067,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="57" t="s">
         <v>31</v>
       </c>
@@ -3081,7 +3081,7 @@
       <c r="G115" s="85"/>
       <c r="H115" s="85"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="60" t="s">
         <v>33</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="G116" s="8"/>
       <c r="H116" s="62"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="60"/>
       <c r="B117" s="8"/>
       <c r="C117" s="63">
@@ -3115,7 +3115,7 @@
       <c r="G117" s="8"/>
       <c r="H117" s="62"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="60"/>
       <c r="B118" s="8"/>
       <c r="C118" s="63"/>
@@ -3125,7 +3125,7 @@
       <c r="G118" s="8"/>
       <c r="H118" s="62"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="86" t="s">
         <v>37</v>
       </c>
@@ -3137,7 +3137,7 @@
       <c r="G119" s="86"/>
       <c r="H119" s="86"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="87" t="s">
         <v>38</v>
       </c>
@@ -3149,7 +3149,7 @@
       <c r="G120" s="87"/>
       <c r="H120" s="87"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="87"/>
       <c r="B121" s="87"/>
       <c r="C121" s="87"/>
@@ -3159,7 +3159,7 @@
       <c r="G121" s="87"/>
       <c r="H121" s="87"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="87"/>
       <c r="B122" s="87"/>
       <c r="C122" s="87"/>
@@ -3169,7 +3169,7 @@
       <c r="G122" s="87"/>
       <c r="H122" s="87"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="87"/>
       <c r="B123" s="87"/>
       <c r="C123" s="87"/>
@@ -3179,7 +3179,7 @@
       <c r="G123" s="87"/>
       <c r="H123" s="87"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="87"/>
       <c r="B124" s="87"/>
       <c r="C124" s="87"/>
@@ -3189,7 +3189,7 @@
       <c r="G124" s="87"/>
       <c r="H124" s="87"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="60"/>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
@@ -3203,7 +3203,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="60" t="s">
         <v>41</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="60"/>
       <c r="B127" s="8"/>
       <c r="C127" s="61"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="H127" s="77"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="60"/>
       <c r="B128" s="8"/>
       <c r="C128" s="61"/>
@@ -3241,7 +3241,7 @@
       <c r="G128" s="76"/>
       <c r="H128" s="78"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="60" t="s">
         <v>33</v>
       </c>
@@ -3259,7 +3259,7 @@
       <c r="G129" s="76"/>
       <c r="H129" s="79"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="80"/>
       <c r="B130" s="81"/>
       <c r="C130" s="82" t="s">
@@ -3284,54 +3284,642 @@
     <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B136" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C136" s="85"/>
+      <c r="D136" s="85"/>
+      <c r="E136" s="85"/>
+      <c r="F136" s="85"/>
+      <c r="G136" s="85"/>
+      <c r="H136" s="85"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B137" s="8"/>
+      <c r="C137" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D137" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E137" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="62"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="60"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="63">
+        <v>59</v>
+      </c>
+      <c r="D138" s="63">
+        <v>5</v>
+      </c>
+      <c r="E138" s="63">
+        <v>1</v>
+      </c>
+      <c r="F138" s="8"/>
+      <c r="G138" s="8"/>
+      <c r="H138" s="62"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="60"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="63"/>
+      <c r="D139" s="63"/>
+      <c r="E139" s="63"/>
+      <c r="F139" s="8"/>
+      <c r="G139" s="8"/>
+      <c r="H139" s="62"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B140" s="86"/>
+      <c r="C140" s="86"/>
+      <c r="D140" s="86"/>
+      <c r="E140" s="86"/>
+      <c r="F140" s="86"/>
+      <c r="G140" s="86"/>
+      <c r="H140" s="86"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B141" s="87"/>
+      <c r="C141" s="87"/>
+      <c r="D141" s="87"/>
+      <c r="E141" s="87"/>
+      <c r="F141" s="87"/>
+      <c r="G141" s="87"/>
+      <c r="H141" s="87"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="87"/>
+      <c r="B142" s="87"/>
+      <c r="C142" s="87"/>
+      <c r="D142" s="87"/>
+      <c r="E142" s="87"/>
+      <c r="F142" s="87"/>
+      <c r="G142" s="87"/>
+      <c r="H142" s="87"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="87"/>
+      <c r="B143" s="87"/>
+      <c r="C143" s="87"/>
+      <c r="D143" s="87"/>
+      <c r="E143" s="87"/>
+      <c r="F143" s="87"/>
+      <c r="G143" s="87"/>
+      <c r="H143" s="87"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="87"/>
+      <c r="B144" s="87"/>
+      <c r="C144" s="87"/>
+      <c r="D144" s="87"/>
+      <c r="E144" s="87"/>
+      <c r="F144" s="87"/>
+      <c r="G144" s="87"/>
+      <c r="H144" s="87"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="87"/>
+      <c r="B145" s="87"/>
+      <c r="C145" s="87"/>
+      <c r="D145" s="87"/>
+      <c r="E145" s="87"/>
+      <c r="F145" s="87"/>
+      <c r="G145" s="87"/>
+      <c r="H145" s="87"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="60"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+      <c r="F146" s="8"/>
+      <c r="G146" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H146" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B147" s="8"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="75"/>
+      <c r="G147" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H147" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="60"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="61"/>
+      <c r="D148" s="61"/>
+      <c r="E148" s="61"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H148" s="77"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="60"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="61"/>
+      <c r="D149" s="61"/>
+      <c r="E149" s="61"/>
+      <c r="F149" s="8"/>
+      <c r="G149" s="76"/>
+      <c r="H149" s="78"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B150" s="8"/>
+      <c r="C150" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D150" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E150" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F150" s="8"/>
+      <c r="G150" s="76"/>
+      <c r="H150" s="79"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="80"/>
+      <c r="B151" s="81"/>
+      <c r="C151" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D151" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E151" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F151" s="81"/>
+      <c r="G151" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H151" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B152" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C152" s="85"/>
+      <c r="D152" s="85"/>
+      <c r="E152" s="85"/>
+      <c r="F152" s="85"/>
+      <c r="G152" s="85"/>
+      <c r="H152" s="85"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B153" s="8"/>
+      <c r="C153" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D153" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E153" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F153" s="8"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="62"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="60"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="63">
+        <v>64</v>
+      </c>
+      <c r="D154" s="63">
+        <v>2</v>
+      </c>
+      <c r="E154" s="63">
+        <v>1</v>
+      </c>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="62"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="60"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="63"/>
+      <c r="D155" s="63"/>
+      <c r="E155" s="63"/>
+      <c r="F155" s="8"/>
+      <c r="G155" s="8"/>
+      <c r="H155" s="62"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B156" s="86"/>
+      <c r="C156" s="86"/>
+      <c r="D156" s="86"/>
+      <c r="E156" s="86"/>
+      <c r="F156" s="86"/>
+      <c r="G156" s="86"/>
+      <c r="H156" s="86"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B157" s="87"/>
+      <c r="C157" s="87"/>
+      <c r="D157" s="87"/>
+      <c r="E157" s="87"/>
+      <c r="F157" s="87"/>
+      <c r="G157" s="87"/>
+      <c r="H157" s="87"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="87"/>
+      <c r="B158" s="87"/>
+      <c r="C158" s="87"/>
+      <c r="D158" s="87"/>
+      <c r="E158" s="87"/>
+      <c r="F158" s="87"/>
+      <c r="G158" s="87"/>
+      <c r="H158" s="87"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="87"/>
+      <c r="B159" s="87"/>
+      <c r="C159" s="87"/>
+      <c r="D159" s="87"/>
+      <c r="E159" s="87"/>
+      <c r="F159" s="87"/>
+      <c r="G159" s="87"/>
+      <c r="H159" s="87"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="87"/>
+      <c r="B160" s="87"/>
+      <c r="C160" s="87"/>
+      <c r="D160" s="87"/>
+      <c r="E160" s="87"/>
+      <c r="F160" s="87"/>
+      <c r="G160" s="87"/>
+      <c r="H160" s="87"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="87"/>
+      <c r="B161" s="87"/>
+      <c r="C161" s="87"/>
+      <c r="D161" s="87"/>
+      <c r="E161" s="87"/>
+      <c r="F161" s="87"/>
+      <c r="G161" s="87"/>
+      <c r="H161" s="87"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" s="60"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
+      <c r="F162" s="8"/>
+      <c r="G162" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H162" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B163" s="8"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="75"/>
+      <c r="G163" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H163" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="60"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="61"/>
+      <c r="D164" s="61"/>
+      <c r="E164" s="61"/>
+      <c r="F164" s="8"/>
+      <c r="G164" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H164" s="77"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="60"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="61"/>
+      <c r="D165" s="61"/>
+      <c r="E165" s="61"/>
+      <c r="F165" s="8"/>
+      <c r="G165" s="76"/>
+      <c r="H165" s="78"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B166" s="8"/>
+      <c r="C166" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D166" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E166" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F166" s="8"/>
+      <c r="G166" s="76"/>
+      <c r="H166" s="79"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="80"/>
+      <c r="B167" s="81"/>
+      <c r="C167" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D167" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E167" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F167" s="81"/>
+      <c r="G167" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H167" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B168" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C168" s="85"/>
+      <c r="D168" s="85"/>
+      <c r="E168" s="85"/>
+      <c r="F168" s="85"/>
+      <c r="G168" s="85"/>
+      <c r="H168" s="85"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B169" s="8"/>
+      <c r="C169" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D169" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E169" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F169" s="8"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="62"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="60"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="63">
+        <v>66</v>
+      </c>
+      <c r="D170" s="63">
+        <v>3</v>
+      </c>
+      <c r="E170" s="63">
+        <v>0</v>
+      </c>
+      <c r="F170" s="8"/>
+      <c r="G170" s="8"/>
+      <c r="H170" s="62"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171" s="60"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="63"/>
+      <c r="D171" s="63"/>
+      <c r="E171" s="63"/>
+      <c r="F171" s="8"/>
+      <c r="G171" s="8"/>
+      <c r="H171" s="62"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B172" s="86"/>
+      <c r="C172" s="86"/>
+      <c r="D172" s="86"/>
+      <c r="E172" s="86"/>
+      <c r="F172" s="86"/>
+      <c r="G172" s="86"/>
+      <c r="H172" s="86"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B173" s="87"/>
+      <c r="C173" s="87"/>
+      <c r="D173" s="87"/>
+      <c r="E173" s="87"/>
+      <c r="F173" s="87"/>
+      <c r="G173" s="87"/>
+      <c r="H173" s="87"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174" s="87"/>
+      <c r="B174" s="87"/>
+      <c r="C174" s="87"/>
+      <c r="D174" s="87"/>
+      <c r="E174" s="87"/>
+      <c r="F174" s="87"/>
+      <c r="G174" s="87"/>
+      <c r="H174" s="87"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" s="87"/>
+      <c r="B175" s="87"/>
+      <c r="C175" s="87"/>
+      <c r="D175" s="87"/>
+      <c r="E175" s="87"/>
+      <c r="F175" s="87"/>
+      <c r="G175" s="87"/>
+      <c r="H175" s="87"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" s="87"/>
+      <c r="B176" s="87"/>
+      <c r="C176" s="87"/>
+      <c r="D176" s="87"/>
+      <c r="E176" s="87"/>
+      <c r="F176" s="87"/>
+      <c r="G176" s="87"/>
+      <c r="H176" s="87"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="87"/>
+      <c r="B177" s="87"/>
+      <c r="C177" s="87"/>
+      <c r="D177" s="87"/>
+      <c r="E177" s="87"/>
+      <c r="F177" s="87"/>
+      <c r="G177" s="87"/>
+      <c r="H177" s="87"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="60"/>
+      <c r="B178" s="8"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+      <c r="E178" s="8"/>
+      <c r="F178" s="8"/>
+      <c r="G178" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H178" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B179" s="8"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="7"/>
+      <c r="F179" s="75"/>
+      <c r="G179" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H179" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="60"/>
+      <c r="B180" s="8"/>
+      <c r="C180" s="61"/>
+      <c r="D180" s="61"/>
+      <c r="E180" s="61"/>
+      <c r="F180" s="8"/>
+      <c r="G180" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H180" s="77"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181" s="60"/>
+      <c r="B181" s="8"/>
+      <c r="C181" s="61"/>
+      <c r="D181" s="61"/>
+      <c r="E181" s="61"/>
+      <c r="F181" s="8"/>
+      <c r="G181" s="76"/>
+      <c r="H181" s="78"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B182" s="8"/>
+      <c r="C182" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D182" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E182" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F182" s="8"/>
+      <c r="G182" s="76"/>
+      <c r="H182" s="79"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="80"/>
+      <c r="B183" s="81"/>
+      <c r="C183" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D183" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E183" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F183" s="81"/>
+      <c r="G183" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H183" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
@@ -3398,7 +3986,7 @@
     <row r="247" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="42">
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
@@ -3432,6 +4020,15 @@
     <mergeCell ref="B115:H115"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="A120:H124"/>
+    <mergeCell ref="B136:H136"/>
+    <mergeCell ref="A140:H140"/>
+    <mergeCell ref="A141:H145"/>
+    <mergeCell ref="B152:H152"/>
+    <mergeCell ref="A156:H156"/>
+    <mergeCell ref="A157:H161"/>
+    <mergeCell ref="B168:H168"/>
+    <mergeCell ref="A172:H172"/>
+    <mergeCell ref="A173:H177"/>
   </mergeCells>
   <conditionalFormatting sqref="A28">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">

</xml_diff>

<commit_message>
Separate PAX button loading states and improve update functionality
Refactors the client-side logic for PAX report updates, separating the loading states for the "Update PAX" and "Update Existing PAX" buttons, and introduces a new success modal for the updated PAX report.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a3af5c32-fe94-463b-bafd-8d7cf4140d74
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d67b414c-7ba7-46ed-90da-331e0aa9efb6/a3af5c32-fe94-463b-bafd-8d7cf4140d74/JjpQe9e
</commit_message>
<xml_diff>
--- a/output/ship-b/eod_1757671798062.xlsx
+++ b/output/ship-b/eod_1757671798062.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="56">
   <si>
     <t>TOUR OPERATOR REPORT</t>
   </si>
@@ -3284,7 +3284,7 @@
     <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="57" t="s">
         <v>31</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="G136" s="85"/>
       <c r="H136" s="85"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="60" t="s">
         <v>33</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="G137" s="8"/>
       <c r="H137" s="62"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="60"/>
       <c r="B138" s="8"/>
       <c r="C138" s="63">
@@ -3332,7 +3332,7 @@
       <c r="G138" s="8"/>
       <c r="H138" s="62"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="60"/>
       <c r="B139" s="8"/>
       <c r="C139" s="63"/>
@@ -3342,7 +3342,7 @@
       <c r="G139" s="8"/>
       <c r="H139" s="62"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="86" t="s">
         <v>37</v>
       </c>
@@ -3354,7 +3354,7 @@
       <c r="G140" s="86"/>
       <c r="H140" s="86"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="87" t="s">
         <v>38</v>
       </c>
@@ -3366,7 +3366,7 @@
       <c r="G141" s="87"/>
       <c r="H141" s="87"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="87"/>
       <c r="B142" s="87"/>
       <c r="C142" s="87"/>
@@ -3376,7 +3376,7 @@
       <c r="G142" s="87"/>
       <c r="H142" s="87"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="87"/>
       <c r="B143" s="87"/>
       <c r="C143" s="87"/>
@@ -3386,7 +3386,7 @@
       <c r="G143" s="87"/>
       <c r="H143" s="87"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="87"/>
       <c r="B144" s="87"/>
       <c r="C144" s="87"/>
@@ -3396,7 +3396,7 @@
       <c r="G144" s="87"/>
       <c r="H144" s="87"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="87"/>
       <c r="B145" s="87"/>
       <c r="C145" s="87"/>
@@ -3406,7 +3406,7 @@
       <c r="G145" s="87"/>
       <c r="H145" s="87"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="60"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
@@ -3420,7 +3420,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="60" t="s">
         <v>41</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="60"/>
       <c r="B148" s="8"/>
       <c r="C148" s="61"/>
@@ -3448,7 +3448,7 @@
       </c>
       <c r="H148" s="77"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="60"/>
       <c r="B149" s="8"/>
       <c r="C149" s="61"/>
@@ -3458,7 +3458,7 @@
       <c r="G149" s="76"/>
       <c r="H149" s="78"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="60" t="s">
         <v>33</v>
       </c>
@@ -3476,7 +3476,7 @@
       <c r="G150" s="76"/>
       <c r="H150" s="79"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="80"/>
       <c r="B151" s="81"/>
       <c r="C151" s="82" t="s">
@@ -3496,7 +3496,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="57" t="s">
         <v>31</v>
       </c>
@@ -3510,7 +3510,7 @@
       <c r="G152" s="85"/>
       <c r="H152" s="85"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="60" t="s">
         <v>33</v>
       </c>
@@ -3528,7 +3528,7 @@
       <c r="G153" s="8"/>
       <c r="H153" s="62"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="60"/>
       <c r="B154" s="8"/>
       <c r="C154" s="63">
@@ -3544,7 +3544,7 @@
       <c r="G154" s="8"/>
       <c r="H154" s="62"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="60"/>
       <c r="B155" s="8"/>
       <c r="C155" s="63"/>
@@ -3554,7 +3554,7 @@
       <c r="G155" s="8"/>
       <c r="H155" s="62"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="86" t="s">
         <v>37</v>
       </c>
@@ -3566,7 +3566,7 @@
       <c r="G156" s="86"/>
       <c r="H156" s="86"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="87" t="s">
         <v>52</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="G157" s="87"/>
       <c r="H157" s="87"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="87"/>
       <c r="B158" s="87"/>
       <c r="C158" s="87"/>
@@ -3588,7 +3588,7 @@
       <c r="G158" s="87"/>
       <c r="H158" s="87"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="87"/>
       <c r="B159" s="87"/>
       <c r="C159" s="87"/>
@@ -3598,7 +3598,7 @@
       <c r="G159" s="87"/>
       <c r="H159" s="87"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="87"/>
       <c r="B160" s="87"/>
       <c r="C160" s="87"/>
@@ -3608,7 +3608,7 @@
       <c r="G160" s="87"/>
       <c r="H160" s="87"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="87"/>
       <c r="B161" s="87"/>
       <c r="C161" s="87"/>
@@ -3618,7 +3618,7 @@
       <c r="G161" s="87"/>
       <c r="H161" s="87"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="60"/>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
@@ -3632,7 +3632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="60" t="s">
         <v>41</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="60"/>
       <c r="B164" s="8"/>
       <c r="C164" s="61"/>
@@ -3660,7 +3660,7 @@
       </c>
       <c r="H164" s="77"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="60"/>
       <c r="B165" s="8"/>
       <c r="C165" s="61"/>
@@ -3670,7 +3670,7 @@
       <c r="G165" s="76"/>
       <c r="H165" s="78"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="60" t="s">
         <v>33</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="G166" s="76"/>
       <c r="H166" s="79"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="80"/>
       <c r="B167" s="81"/>
       <c r="C167" s="82" t="s">
@@ -3708,7 +3708,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="57" t="s">
         <v>31</v>
       </c>
@@ -3722,7 +3722,7 @@
       <c r="G168" s="85"/>
       <c r="H168" s="85"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="60" t="s">
         <v>33</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="G169" s="8"/>
       <c r="H169" s="62"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="60"/>
       <c r="B170" s="8"/>
       <c r="C170" s="63">
@@ -3756,7 +3756,7 @@
       <c r="G170" s="8"/>
       <c r="H170" s="62"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="60"/>
       <c r="B171" s="8"/>
       <c r="C171" s="63"/>
@@ -3766,7 +3766,7 @@
       <c r="G171" s="8"/>
       <c r="H171" s="62"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="86" t="s">
         <v>37</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="G172" s="86"/>
       <c r="H172" s="86"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="87" t="s">
         <v>38</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="G173" s="87"/>
       <c r="H173" s="87"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="87"/>
       <c r="B174" s="87"/>
       <c r="C174" s="87"/>
@@ -3800,7 +3800,7 @@
       <c r="G174" s="87"/>
       <c r="H174" s="87"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="87"/>
       <c r="B175" s="87"/>
       <c r="C175" s="87"/>
@@ -3810,7 +3810,7 @@
       <c r="G175" s="87"/>
       <c r="H175" s="87"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="87"/>
       <c r="B176" s="87"/>
       <c r="C176" s="87"/>
@@ -3820,7 +3820,7 @@
       <c r="G176" s="87"/>
       <c r="H176" s="87"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="87"/>
       <c r="B177" s="87"/>
       <c r="C177" s="87"/>
@@ -3830,7 +3830,7 @@
       <c r="G177" s="87"/>
       <c r="H177" s="87"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="60"/>
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
@@ -3844,7 +3844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="60" t="s">
         <v>41</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="60"/>
       <c r="B180" s="8"/>
       <c r="C180" s="61"/>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="H180" s="77"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="60"/>
       <c r="B181" s="8"/>
       <c r="C181" s="61"/>
@@ -3882,7 +3882,7 @@
       <c r="G181" s="76"/>
       <c r="H181" s="78"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="60" t="s">
         <v>33</v>
       </c>
@@ -3900,7 +3900,7 @@
       <c r="G182" s="76"/>
       <c r="H182" s="79"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="80"/>
       <c r="B183" s="81"/>
       <c r="C183" s="82" t="s">
@@ -3925,54 +3925,642 @@
     <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B189" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C189" s="85"/>
+      <c r="D189" s="85"/>
+      <c r="E189" s="85"/>
+      <c r="F189" s="85"/>
+      <c r="G189" s="85"/>
+      <c r="H189" s="85"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B190" s="8"/>
+      <c r="C190" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D190" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E190" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F190" s="8"/>
+      <c r="G190" s="8"/>
+      <c r="H190" s="62"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="60"/>
+      <c r="B191" s="8"/>
+      <c r="C191" s="63">
+        <v>89</v>
+      </c>
+      <c r="D191" s="63">
+        <v>5</v>
+      </c>
+      <c r="E191" s="63">
+        <v>1</v>
+      </c>
+      <c r="F191" s="8"/>
+      <c r="G191" s="8"/>
+      <c r="H191" s="62"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" s="60"/>
+      <c r="B192" s="8"/>
+      <c r="C192" s="63"/>
+      <c r="D192" s="63"/>
+      <c r="E192" s="63"/>
+      <c r="F192" s="8"/>
+      <c r="G192" s="8"/>
+      <c r="H192" s="62"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B193" s="86"/>
+      <c r="C193" s="86"/>
+      <c r="D193" s="86"/>
+      <c r="E193" s="86"/>
+      <c r="F193" s="86"/>
+      <c r="G193" s="86"/>
+      <c r="H193" s="86"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B194" s="87"/>
+      <c r="C194" s="87"/>
+      <c r="D194" s="87"/>
+      <c r="E194" s="87"/>
+      <c r="F194" s="87"/>
+      <c r="G194" s="87"/>
+      <c r="H194" s="87"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="87"/>
+      <c r="B195" s="87"/>
+      <c r="C195" s="87"/>
+      <c r="D195" s="87"/>
+      <c r="E195" s="87"/>
+      <c r="F195" s="87"/>
+      <c r="G195" s="87"/>
+      <c r="H195" s="87"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="87"/>
+      <c r="B196" s="87"/>
+      <c r="C196" s="87"/>
+      <c r="D196" s="87"/>
+      <c r="E196" s="87"/>
+      <c r="F196" s="87"/>
+      <c r="G196" s="87"/>
+      <c r="H196" s="87"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="87"/>
+      <c r="B197" s="87"/>
+      <c r="C197" s="87"/>
+      <c r="D197" s="87"/>
+      <c r="E197" s="87"/>
+      <c r="F197" s="87"/>
+      <c r="G197" s="87"/>
+      <c r="H197" s="87"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="87"/>
+      <c r="B198" s="87"/>
+      <c r="C198" s="87"/>
+      <c r="D198" s="87"/>
+      <c r="E198" s="87"/>
+      <c r="F198" s="87"/>
+      <c r="G198" s="87"/>
+      <c r="H198" s="87"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="60"/>
+      <c r="B199" s="8"/>
+      <c r="C199" s="8"/>
+      <c r="D199" s="8"/>
+      <c r="E199" s="8"/>
+      <c r="F199" s="8"/>
+      <c r="G199" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H199" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B200" s="8"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="7"/>
+      <c r="E200" s="7"/>
+      <c r="F200" s="75"/>
+      <c r="G200" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H200" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="60"/>
+      <c r="B201" s="8"/>
+      <c r="C201" s="61"/>
+      <c r="D201" s="61"/>
+      <c r="E201" s="61"/>
+      <c r="F201" s="8"/>
+      <c r="G201" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H201" s="77"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" s="60"/>
+      <c r="B202" s="8"/>
+      <c r="C202" s="61"/>
+      <c r="D202" s="61"/>
+      <c r="E202" s="61"/>
+      <c r="F202" s="8"/>
+      <c r="G202" s="76"/>
+      <c r="H202" s="78"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B203" s="8"/>
+      <c r="C203" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D203" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E203" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F203" s="8"/>
+      <c r="G203" s="76"/>
+      <c r="H203" s="79"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="80"/>
+      <c r="B204" s="81"/>
+      <c r="C204" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D204" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E204" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F204" s="81"/>
+      <c r="G204" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H204" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B205" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C205" s="85"/>
+      <c r="D205" s="85"/>
+      <c r="E205" s="85"/>
+      <c r="F205" s="85"/>
+      <c r="G205" s="85"/>
+      <c r="H205" s="85"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B206" s="8"/>
+      <c r="C206" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D206" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E206" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F206" s="8"/>
+      <c r="G206" s="8"/>
+      <c r="H206" s="62"/>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="60"/>
+      <c r="B207" s="8"/>
+      <c r="C207" s="63">
+        <v>92</v>
+      </c>
+      <c r="D207" s="63">
+        <v>2</v>
+      </c>
+      <c r="E207" s="63">
+        <v>1</v>
+      </c>
+      <c r="F207" s="8"/>
+      <c r="G207" s="8"/>
+      <c r="H207" s="62"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="60"/>
+      <c r="B208" s="8"/>
+      <c r="C208" s="63"/>
+      <c r="D208" s="63"/>
+      <c r="E208" s="63"/>
+      <c r="F208" s="8"/>
+      <c r="G208" s="8"/>
+      <c r="H208" s="62"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B209" s="86"/>
+      <c r="C209" s="86"/>
+      <c r="D209" s="86"/>
+      <c r="E209" s="86"/>
+      <c r="F209" s="86"/>
+      <c r="G209" s="86"/>
+      <c r="H209" s="86"/>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B210" s="87"/>
+      <c r="C210" s="87"/>
+      <c r="D210" s="87"/>
+      <c r="E210" s="87"/>
+      <c r="F210" s="87"/>
+      <c r="G210" s="87"/>
+      <c r="H210" s="87"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A211" s="87"/>
+      <c r="B211" s="87"/>
+      <c r="C211" s="87"/>
+      <c r="D211" s="87"/>
+      <c r="E211" s="87"/>
+      <c r="F211" s="87"/>
+      <c r="G211" s="87"/>
+      <c r="H211" s="87"/>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212" s="87"/>
+      <c r="B212" s="87"/>
+      <c r="C212" s="87"/>
+      <c r="D212" s="87"/>
+      <c r="E212" s="87"/>
+      <c r="F212" s="87"/>
+      <c r="G212" s="87"/>
+      <c r="H212" s="87"/>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213" s="87"/>
+      <c r="B213" s="87"/>
+      <c r="C213" s="87"/>
+      <c r="D213" s="87"/>
+      <c r="E213" s="87"/>
+      <c r="F213" s="87"/>
+      <c r="G213" s="87"/>
+      <c r="H213" s="87"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214" s="87"/>
+      <c r="B214" s="87"/>
+      <c r="C214" s="87"/>
+      <c r="D214" s="87"/>
+      <c r="E214" s="87"/>
+      <c r="F214" s="87"/>
+      <c r="G214" s="87"/>
+      <c r="H214" s="87"/>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="60"/>
+      <c r="B215" s="8"/>
+      <c r="C215" s="8"/>
+      <c r="D215" s="8"/>
+      <c r="E215" s="8"/>
+      <c r="F215" s="8"/>
+      <c r="G215" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H215" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B216" s="8"/>
+      <c r="C216" s="7"/>
+      <c r="D216" s="7"/>
+      <c r="E216" s="7"/>
+      <c r="F216" s="75"/>
+      <c r="G216" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H216" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" s="60"/>
+      <c r="B217" s="8"/>
+      <c r="C217" s="61"/>
+      <c r="D217" s="61"/>
+      <c r="E217" s="61"/>
+      <c r="F217" s="8"/>
+      <c r="G217" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H217" s="77"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="60"/>
+      <c r="B218" s="8"/>
+      <c r="C218" s="61"/>
+      <c r="D218" s="61"/>
+      <c r="E218" s="61"/>
+      <c r="F218" s="8"/>
+      <c r="G218" s="76"/>
+      <c r="H218" s="78"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B219" s="8"/>
+      <c r="C219" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D219" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E219" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F219" s="8"/>
+      <c r="G219" s="76"/>
+      <c r="H219" s="79"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220" s="80"/>
+      <c r="B220" s="81"/>
+      <c r="C220" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D220" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E220" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F220" s="81"/>
+      <c r="G220" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H220" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B221" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C221" s="85"/>
+      <c r="D221" s="85"/>
+      <c r="E221" s="85"/>
+      <c r="F221" s="85"/>
+      <c r="G221" s="85"/>
+      <c r="H221" s="85"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B222" s="8"/>
+      <c r="C222" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D222" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E222" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F222" s="8"/>
+      <c r="G222" s="8"/>
+      <c r="H222" s="62"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="60"/>
+      <c r="B223" s="8"/>
+      <c r="C223" s="63">
+        <v>102</v>
+      </c>
+      <c r="D223" s="63">
+        <v>3</v>
+      </c>
+      <c r="E223" s="63">
+        <v>0</v>
+      </c>
+      <c r="F223" s="8"/>
+      <c r="G223" s="8"/>
+      <c r="H223" s="62"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A224" s="60"/>
+      <c r="B224" s="8"/>
+      <c r="C224" s="63"/>
+      <c r="D224" s="63"/>
+      <c r="E224" s="63"/>
+      <c r="F224" s="8"/>
+      <c r="G224" s="8"/>
+      <c r="H224" s="62"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A225" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B225" s="86"/>
+      <c r="C225" s="86"/>
+      <c r="D225" s="86"/>
+      <c r="E225" s="86"/>
+      <c r="F225" s="86"/>
+      <c r="G225" s="86"/>
+      <c r="H225" s="86"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A226" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="B226" s="87"/>
+      <c r="C226" s="87"/>
+      <c r="D226" s="87"/>
+      <c r="E226" s="87"/>
+      <c r="F226" s="87"/>
+      <c r="G226" s="87"/>
+      <c r="H226" s="87"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A227" s="87"/>
+      <c r="B227" s="87"/>
+      <c r="C227" s="87"/>
+      <c r="D227" s="87"/>
+      <c r="E227" s="87"/>
+      <c r="F227" s="87"/>
+      <c r="G227" s="87"/>
+      <c r="H227" s="87"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A228" s="87"/>
+      <c r="B228" s="87"/>
+      <c r="C228" s="87"/>
+      <c r="D228" s="87"/>
+      <c r="E228" s="87"/>
+      <c r="F228" s="87"/>
+      <c r="G228" s="87"/>
+      <c r="H228" s="87"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" s="87"/>
+      <c r="B229" s="87"/>
+      <c r="C229" s="87"/>
+      <c r="D229" s="87"/>
+      <c r="E229" s="87"/>
+      <c r="F229" s="87"/>
+      <c r="G229" s="87"/>
+      <c r="H229" s="87"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230" s="87"/>
+      <c r="B230" s="87"/>
+      <c r="C230" s="87"/>
+      <c r="D230" s="87"/>
+      <c r="E230" s="87"/>
+      <c r="F230" s="87"/>
+      <c r="G230" s="87"/>
+      <c r="H230" s="87"/>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A231" s="60"/>
+      <c r="B231" s="8"/>
+      <c r="C231" s="8"/>
+      <c r="D231" s="8"/>
+      <c r="E231" s="8"/>
+      <c r="F231" s="8"/>
+      <c r="G231" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H231" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B232" s="8"/>
+      <c r="C232" s="7"/>
+      <c r="D232" s="7"/>
+      <c r="E232" s="7"/>
+      <c r="F232" s="75"/>
+      <c r="G232" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="H232" s="74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233" s="60"/>
+      <c r="B233" s="8"/>
+      <c r="C233" s="61"/>
+      <c r="D233" s="61"/>
+      <c r="E233" s="61"/>
+      <c r="F233" s="8"/>
+      <c r="G233" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H233" s="77"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234" s="60"/>
+      <c r="B234" s="8"/>
+      <c r="C234" s="61"/>
+      <c r="D234" s="61"/>
+      <c r="E234" s="61"/>
+      <c r="F234" s="8"/>
+      <c r="G234" s="76"/>
+      <c r="H234" s="78"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B235" s="8"/>
+      <c r="C235" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D235" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E235" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F235" s="8"/>
+      <c r="G235" s="76"/>
+      <c r="H235" s="79"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A236" s="80"/>
+      <c r="B236" s="81"/>
+      <c r="C236" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D236" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E236" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F236" s="81"/>
+      <c r="G236" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H236" s="84" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25"/>
@@ -3986,7 +4574,7 @@
     <row r="247" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="51">
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C5:H5"/>
@@ -4029,6 +4617,15 @@
     <mergeCell ref="B168:H168"/>
     <mergeCell ref="A172:H172"/>
     <mergeCell ref="A173:H177"/>
+    <mergeCell ref="B189:H189"/>
+    <mergeCell ref="A193:H193"/>
+    <mergeCell ref="A194:H198"/>
+    <mergeCell ref="B205:H205"/>
+    <mergeCell ref="A209:H209"/>
+    <mergeCell ref="A210:H214"/>
+    <mergeCell ref="B221:H221"/>
+    <mergeCell ref="A225:H225"/>
+    <mergeCell ref="A226:H230"/>
   </mergeCells>
   <conditionalFormatting sqref="A28">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">

</xml_diff>